<commit_message>
feat: final version of template for the Balance Sheet Report
In service of #10 and #14
</commit_message>
<xml_diff>
--- a/src/Services/Export/ExcelTemplates/BalanceSheetReport.xlsx
+++ b/src/Services/Export/ExcelTemplates/BalanceSheetReport.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DashAccountingSystemV2\src\Services\Export\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B585DB-4491-440F-AC5D-AD088D33AE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFE2476-5CDB-4600-A031-D6E8C63BE044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{53223017-E30C-4245-AF98-818869291275}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="assets">Sheet1!$A$8:$G$9</definedName>
+    <definedName name="equity">Sheet1!$A$20:$G$21</definedName>
+    <definedName name="liabilities">Sheet1!$A$14:$G$15</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>{{tenant.Name}}</t>
   </si>
@@ -49,12 +54,42 @@
   </si>
   <si>
     <t>&amp;="As of " &amp; "{{reportDates.DateRangeEnd}}"</t>
+  </si>
+  <si>
+    <t>{{item.AccountName}}</t>
+  </si>
+  <si>
+    <t>{{item.Balance}}</t>
+  </si>
+  <si>
+    <t>TOTAL ASSETS</t>
+  </si>
+  <si>
+    <t>TOTAL LIABILITIES</t>
+  </si>
+  <si>
+    <t>TOTAL EQUITY</t>
+  </si>
+  <si>
+    <t>LIABILITIES</t>
+  </si>
+  <si>
+    <t>EQUITY</t>
+  </si>
+  <si>
+    <t>TOTAL LIABILITIES &amp; EQUITY</t>
+  </si>
+  <si>
+    <t>&lt;&lt;sum&gt;&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -80,14 +115,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -101,6 +128,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -110,7 +145,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -127,32 +162,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
+    <cellStyle name="Total" xfId="3" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -464,11 +538,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF54718D-068D-49E3-83CB-0A29717394C5}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,67 +552,196 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G5" s="1" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="4" t="e">
+        <f>G$15+G$21</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="13">
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A9:F9"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A18:G18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: substantially complete export infrastructure & Balance Sheet
* Resolves #10
* Resolves #14
</commit_message>
<xml_diff>
--- a/src/Services/Export/ExcelTemplates/BalanceSheetReport.xlsx
+++ b/src/Services/Export/ExcelTemplates/BalanceSheetReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DashAccountingSystemV2\src\Services\Export\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFE2476-5CDB-4600-A031-D6E8C63BE044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F226C90-EC85-42CA-9504-F2C7EED77001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{53223017-E30C-4245-AF98-818869291275}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>{{tenant.Name}}</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>&lt;&lt;sum&gt;&gt;</t>
+  </si>
+  <si>
+    <t>{{reportDateAndMetadata}}</t>
   </si>
 </sst>
 </file>
@@ -90,7 +93,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +134,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -191,7 +201,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -204,6 +214,16 @@
     </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -538,11 +558,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF54718D-068D-49E3-83CB-0A29717394C5}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15:F15"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,43 +572,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="G5" s="3" t="s">
@@ -596,139 +616,168 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
       <c r="G8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
       <c r="G9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
       <c r="G14" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
       <c r="G15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
       <c r="G20" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
       <c r="G21" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
       <c r="G23" s="4" t="e">
         <f>G$15+G$21</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:7" s="5" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="A27:G27"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A6:G6"/>

</xml_diff>

<commit_message>
fix: small stylistic details on Excel Balance Sheet Report Template
* Remove currency symbols from line items and only show them in totals
* Place the cursor in a safe spot up near the top (since, for reasons known only to Microsoft, cursor position is part of the saved state of an Excel file :-)
</commit_message>
<xml_diff>
--- a/src/Services/Export/ExcelTemplates/BalanceSheetReport.xlsx
+++ b/src/Services/Export/ExcelTemplates/BalanceSheetReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DashAccountingSystemV2\src\Services\Export\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F226C90-EC85-42CA-9504-F2C7EED77001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB748BB1-4DD5-41FD-B743-E2128167CCD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{53223017-E30C-4245-AF98-818869291275}"/>
+    <workbookView xWindow="21480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{53223017-E30C-4245-AF98-818869291275}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,8 +90,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -203,9 +204,6 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -220,6 +218,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -611,7 +612,7 @@
       <c r="I3" s="14"/>
     </row>
     <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -636,7 +637,7 @@
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -649,7 +650,7 @@
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -675,7 +676,7 @@
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -688,7 +689,7 @@
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -714,7 +715,7 @@
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -727,7 +728,7 @@
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -741,28 +742,28 @@
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="4" t="e">
+      <c r="G23" s="3" t="e">
         <f>G$15+G$21</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="7"/>
+    <row r="24" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="6"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">

</xml_diff>